<commit_message>
Fixes across the board
</commit_message>
<xml_diff>
--- a/resources/data-imports/Monsters/surface-raid-monsters.xlsx
+++ b/resources/data-imports/Monsters/surface-raid-monsters.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="86">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -215,9 +215,6 @@
   </si>
   <si>
     <t xml:space="preserve">29682215-62106849</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shade Dust</t>
   </si>
   <si>
     <t xml:space="preserve">Corrupted Pirate</t>
@@ -581,13 +578,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AX16"/>
+  <dimension ref="A1:AX15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AS2" activeCellId="0" sqref="AS2:AS15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AE1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AM10" activeCellId="0" sqref="AM10:AN15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.71"/>
@@ -1451,12 +1448,6 @@
       <c r="AL6" s="1" t="n">
         <v>0.348218359120681</v>
       </c>
-      <c r="AM6" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AN6" s="1" t="n">
-        <v>0.01</v>
-      </c>
       <c r="AO6" s="1" t="s">
         <v>53</v>
       </c>
@@ -1484,7 +1475,7 @@
         <v>369</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C7" s="3" t="n">
         <v>157840983.708406</v>
@@ -1550,10 +1541,10 @@
         <v>0</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Z7" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AA7" s="3" t="n">
         <v>157840983.708406</v>
@@ -1592,7 +1583,7 @@
         <v>0.381934253524182</v>
       </c>
       <c r="AM7" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AN7" s="1" t="n">
         <v>0.01</v>
@@ -1624,7 +1615,7 @@
         <v>371</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C8" s="3" t="n">
         <v>228077490.809629</v>
@@ -1690,10 +1681,10 @@
         <v>0</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Z8" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AA8" s="3" t="n">
         <v>228077490.809629</v>
@@ -1732,7 +1723,7 @@
         <v>0.418914655687407</v>
       </c>
       <c r="AM8" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AN8" s="1" t="n">
         <v>0.01</v>
@@ -1764,7 +1755,7 @@
         <v>367</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C9" s="3" t="n">
         <v>329568028.479322</v>
@@ -1830,10 +1821,10 @@
         <v>0</v>
       </c>
       <c r="Y9" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Z9" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AA9" s="3" t="n">
         <v>329568028.479322</v>
@@ -1872,7 +1863,7 @@
         <v>0.459475648309685</v>
       </c>
       <c r="AM9" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AN9" s="1" t="n">
         <v>1</v>
@@ -1904,7 +1895,7 @@
         <v>426</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C10" s="3" t="n">
         <v>476220099.625728</v>
@@ -1970,10 +1961,10 @@
         <v>0</v>
       </c>
       <c r="Y10" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z10" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AA10" s="3" t="n">
         <v>476220099.625728</v>
@@ -2010,12 +2001,6 @@
       </c>
       <c r="AL10" s="1" t="n">
         <v>0.503963918481622</v>
-      </c>
-      <c r="AM10" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AN10" s="1" t="n">
-        <v>1</v>
       </c>
       <c r="AO10" s="1" t="s">
         <v>53</v>
@@ -2044,7 +2029,7 @@
         <v>427</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C11" s="3" t="n">
         <v>688129805.351454</v>
@@ -2110,10 +2095,10 @@
         <v>0</v>
       </c>
       <c r="Y11" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Z11" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AA11" s="3" t="n">
         <v>688129805.351454</v>
@@ -2150,12 +2135,6 @@
       </c>
       <c r="AL11" s="1" t="n">
         <v>0.552759720924687</v>
-      </c>
-      <c r="AM11" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AN11" s="1" t="n">
-        <v>1</v>
       </c>
       <c r="AO11" s="1" t="s">
         <v>53</v>
@@ -2184,7 +2163,7 @@
         <v>428</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C12" s="3" t="n">
         <v>994335664.087218</v>
@@ -2250,10 +2229,10 @@
         <v>0</v>
       </c>
       <c r="Y12" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Z12" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AA12" s="3" t="n">
         <v>994335664.087218</v>
@@ -2290,12 +2269,6 @@
       </c>
       <c r="AL12" s="1" t="n">
         <v>0.606280128143498</v>
-      </c>
-      <c r="AM12" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AN12" s="1" t="n">
-        <v>1</v>
       </c>
       <c r="AO12" s="1" t="s">
         <v>53</v>
@@ -2324,7 +2297,7 @@
         <v>429</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C13" s="3" t="n">
         <v>1436797832.59904</v>
@@ -2390,10 +2363,10 @@
         <v>0</v>
       </c>
       <c r="Y13" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z13" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA13" s="3" t="n">
         <v>1436797832.59904</v>
@@ -2430,12 +2403,6 @@
       </c>
       <c r="AL13" s="1" t="n">
         <v>0.664982595270864</v>
-      </c>
-      <c r="AM13" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AN13" s="1" t="n">
-        <v>1</v>
       </c>
       <c r="AO13" s="1" t="s">
         <v>53</v>
@@ -2464,7 +2431,7 @@
         <v>430</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C14" s="3" t="n">
         <v>2076148011.50311</v>
@@ -2530,10 +2497,10 @@
         <v>0</v>
       </c>
       <c r="Y14" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Z14" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AA14" s="3" t="n">
         <v>2076148011.50311</v>
@@ -2570,12 +2537,6 @@
       </c>
       <c r="AL14" s="1" t="n">
         <v>0.729368870075371</v>
-      </c>
-      <c r="AM14" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AN14" s="1" t="n">
-        <v>1</v>
       </c>
       <c r="AO14" s="1" t="s">
         <v>53</v>
@@ -2604,7 +2565,7 @@
         <v>431</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C15" s="3" t="n">
         <v>2999997959.2614</v>
@@ -2670,10 +2631,10 @@
         <v>0</v>
       </c>
       <c r="Y15" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Z15" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AA15" s="3" t="n">
         <v>2999997959.2614</v>
@@ -2711,12 +2672,6 @@
       <c r="AL15" s="1" t="n">
         <v>0.799989281551548</v>
       </c>
-      <c r="AM15" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AN15" s="1" t="n">
-        <v>1</v>
-      </c>
       <c r="AO15" s="1" t="s">
         <v>53</v>
       </c>
@@ -2738,9 +2693,6 @@
       <c r="AW15" s="1" t="n">
         <v>0.649994455412477</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>